<commit_message>
update metallicity for the sample from HERACLES
</commit_message>
<xml_diff>
--- a/data/nearby.xlsx
+++ b/data/nearby.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="5380" windowWidth="33600" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="37960" yWindow="0" windowWidth="33600" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SGP.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="463">
   <si>
     <t>Galaxy</t>
   </si>
@@ -1254,14 +1254,167 @@
     <t>-0.17</t>
   </si>
   <si>
-    <t>7.30</t>
+    <t>2008A&amp;A...490..555B</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>Walter:2008bq</t>
+  </si>
+  <si>
+    <t>8.69</t>
+  </si>
+  <si>
+    <t>Skillman:1989kg</t>
+  </si>
+  <si>
+    <t>8.16</t>
+  </si>
+  <si>
+    <t>7.76</t>
+  </si>
+  <si>
+    <t>9.28</t>
+  </si>
+  <si>
+    <t>-0.42</t>
+  </si>
+  <si>
+    <t>8.74</t>
+  </si>
+  <si>
+    <t>StorchiBergmann:1994cw</t>
+  </si>
+  <si>
+    <t>8.14</t>
+  </si>
+  <si>
+    <t>9.00</t>
+  </si>
+  <si>
+    <t>8.47</t>
+  </si>
+  <si>
+    <t>-0.54</t>
+  </si>
+  <si>
+    <t>8.56</t>
+  </si>
+  <si>
+    <t>-0.46</t>
+  </si>
+  <si>
+    <t>Moustakas:2006jo</t>
+  </si>
+  <si>
+    <t>7.65</t>
+  </si>
+  <si>
+    <t>7.34</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>9.39</t>
+  </si>
+  <si>
+    <t>-1.52</t>
+  </si>
+  <si>
+    <t>9.19</t>
+  </si>
+  <si>
+    <t>2004ApJ...604..176S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kim et al. 1998 </t>
+  </si>
+  <si>
+    <t>9.25</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Pignatelli:2001ca</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>NED</t>
+  </si>
+  <si>
+    <t>9.08</t>
+  </si>
+  <si>
+    <t>8.49</t>
+  </si>
+  <si>
+    <t>9.01</t>
+  </si>
+  <si>
+    <t>8.44</t>
+  </si>
+  <si>
+    <t>9.17</t>
+  </si>
+  <si>
+    <t>Prieto:2008hc</t>
+  </si>
+  <si>
+    <t>9.24</t>
+  </si>
+  <si>
+    <t>9.04</t>
+  </si>
+  <si>
+    <t>9.03</t>
+  </si>
+  <si>
+    <t>8.31</t>
+  </si>
+  <si>
+    <t>9.35</t>
+  </si>
+  <si>
+    <t>8.65</t>
+  </si>
+  <si>
+    <t>2008AJ</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>8.40</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>DorsJr:2008kk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1285,6 +1438,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1303,7 +1461,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1445,14 +1603,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1523,6 +1726,28 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1593,6 +1818,28 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1925,10 +2172,10 @@
   <dimension ref="A1:CE53"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="BH20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="BG5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BH1" sqref="BH1"/>
+      <selection pane="bottomRight" activeCell="BP52" sqref="BP52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1947,17 +2194,17 @@
     <col min="13" max="13" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15.1640625" style="1" customWidth="1"/>
     <col min="27" max="27" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="128.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="108" style="1" bestFit="1" customWidth="1"/>
@@ -2504,11 +2751,14 @@
       <c r="G3" s="1">
         <v>-72.628600000000006</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>436</v>
+      </c>
       <c r="N3" s="1" t="s">
-        <v>232</v>
+        <v>372</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>234</v>
+        <v>372</v>
       </c>
       <c r="V3" s="1">
         <v>18973</v>
@@ -2656,14 +2906,14 @@
       <c r="BJ4" s="1">
         <v>8.35</v>
       </c>
-      <c r="BK4" s="1">
-        <v>9.19</v>
+      <c r="BK4" s="1" t="s">
+        <v>438</v>
       </c>
       <c r="BL4" s="1">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="BM4" s="1">
-        <v>8.43</v>
+      <c r="BM4" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="BN4" s="1">
         <v>-0.27</v>
@@ -2721,11 +2971,14 @@
       <c r="L5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N5" s="1">
-        <v>37</v>
-      </c>
-      <c r="O5" s="1">
-        <v>315</v>
+      <c r="M5" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="V5" s="1">
         <v>434.7</v>
@@ -2928,11 +3181,14 @@
       <c r="G6" s="1">
         <v>33.579149999999998</v>
       </c>
-      <c r="N6" s="1">
-        <v>56</v>
-      </c>
-      <c r="O6" s="1">
-        <v>102</v>
+      <c r="M6" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>442</v>
       </c>
       <c r="V6" s="1">
         <v>628.29999999999995</v>
@@ -2976,8 +3232,8 @@
       <c r="BK6" s="1">
         <v>8.91</v>
       </c>
-      <c r="BL6" s="1">
-        <v>0.42</v>
+      <c r="BL6" s="1" t="s">
+        <v>419</v>
       </c>
       <c r="BM6" s="1">
         <v>8.32</v>
@@ -3467,8 +3723,8 @@
       <c r="L9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N9" s="1">
-        <v>39</v>
+      <c r="N9" s="1" t="s">
+        <v>364</v>
       </c>
       <c r="O9" s="1">
         <v>213</v>
@@ -3605,14 +3861,14 @@
       <c r="BJ9" s="1">
         <v>8.5</v>
       </c>
-      <c r="BK9" s="1">
-        <v>9.1199999999999992</v>
+      <c r="BK9" s="1" t="s">
+        <v>418</v>
       </c>
       <c r="BL9" s="1">
         <v>-0.34</v>
       </c>
-      <c r="BM9" s="1">
-        <v>8.52</v>
+      <c r="BM9" s="1" t="s">
+        <v>445</v>
       </c>
       <c r="BN9" s="1">
         <v>-0.34</v>
@@ -3682,8 +3938,11 @@
       <c r="G10" s="1">
         <v>-68.506100000000004</v>
       </c>
+      <c r="M10" s="2" t="s">
+        <v>437</v>
+      </c>
       <c r="N10" s="1" t="s">
-        <v>232</v>
+        <v>354</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>233</v>
@@ -3807,32 +4066,32 @@
       <c r="BE11" s="1">
         <v>0.46</v>
       </c>
-      <c r="BG11" s="1">
-        <v>8.44</v>
-      </c>
-      <c r="BH11" s="1">
-        <v>8.44</v>
-      </c>
-      <c r="BI11" s="1">
-        <v>7.94</v>
-      </c>
-      <c r="BJ11" s="1">
-        <v>7.94</v>
-      </c>
-      <c r="BK11" s="1">
-        <v>8.44</v>
+      <c r="BG11" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="BH11" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="BI11" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="BJ11" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="BK11" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="BL11" s="1">
         <v>0</v>
       </c>
-      <c r="BM11" s="1">
-        <v>7.94</v>
+      <c r="BM11" s="1" t="s">
+        <v>417</v>
       </c>
       <c r="BN11" s="1">
         <v>0</v>
       </c>
       <c r="BO11" s="1" t="s">
-        <v>137</v>
+        <v>415</v>
       </c>
       <c r="BP11" s="1">
         <v>8.19</v>
@@ -4098,26 +4357,26 @@
       <c r="BE14" s="1">
         <v>0.31</v>
       </c>
-      <c r="BG14" s="1">
-        <v>7.59</v>
-      </c>
-      <c r="BH14" s="1">
-        <v>7.59</v>
-      </c>
-      <c r="BI14" s="1">
-        <v>7.3</v>
-      </c>
-      <c r="BJ14" s="1">
-        <v>7.3</v>
-      </c>
-      <c r="BK14" s="1">
-        <v>7.59</v>
+      <c r="BG14" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="BH14" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="BI14" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="BJ14" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="BK14" s="1" t="s">
+        <v>429</v>
       </c>
       <c r="BL14" s="1">
         <v>0</v>
       </c>
       <c r="BM14" s="1" t="s">
-        <v>411</v>
+        <v>430</v>
       </c>
       <c r="BN14" s="1">
         <v>0</v>
@@ -4564,26 +4823,26 @@
       <c r="BF17" s="1">
         <v>-20.76</v>
       </c>
-      <c r="BG17" s="1">
-        <v>8.59</v>
-      </c>
-      <c r="BH17" s="1">
-        <v>8.59</v>
-      </c>
-      <c r="BI17" s="1">
-        <v>8.59</v>
-      </c>
-      <c r="BJ17" s="1">
-        <v>8.59</v>
-      </c>
-      <c r="BK17" s="1">
-        <v>8.59</v>
+      <c r="BG17" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="BH17" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="BI17" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="BJ17" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="BK17" s="1" t="s">
+        <v>414</v>
       </c>
       <c r="BL17" s="1">
         <v>0</v>
       </c>
-      <c r="BM17" s="1">
-        <v>8.59</v>
+      <c r="BM17" s="1" t="s">
+        <v>446</v>
       </c>
       <c r="BN17" s="1">
         <v>0</v>
@@ -4779,32 +5038,32 @@
       <c r="BE19" s="1">
         <v>0.42</v>
       </c>
-      <c r="BG19" s="1">
-        <v>9.1300000000000008</v>
-      </c>
-      <c r="BH19" s="1">
-        <v>9.1300000000000008</v>
-      </c>
-      <c r="BI19" s="1">
-        <v>8.4700000000000006</v>
-      </c>
-      <c r="BJ19" s="1">
-        <v>8.4700000000000006</v>
-      </c>
-      <c r="BK19" s="1">
-        <v>9.1300000000000008</v>
-      </c>
-      <c r="BL19" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM19" s="1">
-        <v>8.4700000000000006</v>
-      </c>
-      <c r="BN19" s="1">
-        <v>0</v>
+      <c r="BG19" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="BH19" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="BI19" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="BJ19" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="BK19" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="BL19" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BM19" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="BN19" s="1" t="s">
+        <v>427</v>
       </c>
       <c r="BO19" s="1" t="s">
-        <v>137</v>
+        <v>428</v>
       </c>
       <c r="BP19" s="1">
         <v>8.8000000000000007</v>
@@ -5068,14 +5327,14 @@
       <c r="BJ21" s="1">
         <v>8.36</v>
       </c>
-      <c r="BK21" s="1">
-        <v>8.98</v>
+      <c r="BK21" s="1" t="s">
+        <v>447</v>
       </c>
       <c r="BL21" s="1">
         <v>0</v>
       </c>
-      <c r="BM21" s="1">
-        <v>8.36</v>
+      <c r="BM21" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="BN21" s="1">
         <v>0</v>
@@ -5265,32 +5524,32 @@
       <c r="BE23" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="BG23" s="1">
-        <v>8.65</v>
-      </c>
-      <c r="BH23" s="1">
-        <v>8.65</v>
-      </c>
-      <c r="BI23" s="1">
-        <v>8.11</v>
-      </c>
-      <c r="BJ23" s="1">
-        <v>8.11</v>
-      </c>
-      <c r="BK23" s="1">
-        <v>8.65</v>
+      <c r="BG23" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="BH23" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="BI23" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="BJ23" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="BK23" s="1" t="s">
+        <v>420</v>
       </c>
       <c r="BL23" s="1">
         <v>0</v>
       </c>
-      <c r="BM23" s="1">
-        <v>8.11</v>
+      <c r="BM23" s="1" t="s">
+        <v>394</v>
       </c>
       <c r="BN23" s="1">
         <v>0</v>
       </c>
       <c r="BO23" s="1" t="s">
-        <v>137</v>
+        <v>421</v>
       </c>
       <c r="BP23" s="1">
         <v>8.3800000000000008</v>
@@ -5958,14 +6217,14 @@
       <c r="BJ27" s="1">
         <v>8.34</v>
       </c>
-      <c r="BK27" s="1">
-        <v>9.1</v>
+      <c r="BK27" s="1" t="s">
+        <v>449</v>
       </c>
       <c r="BL27" s="1">
         <v>-0.66</v>
       </c>
-      <c r="BM27" s="1">
-        <v>8.49</v>
+      <c r="BM27" s="1" t="s">
+        <v>394</v>
       </c>
       <c r="BN27" s="1">
         <v>-0.5</v>
@@ -7526,32 +7785,32 @@
       <c r="BE36" s="1">
         <v>0.53</v>
       </c>
-      <c r="BG36" s="1">
-        <v>8.61</v>
-      </c>
-      <c r="BH36" s="1">
-        <v>8.61</v>
-      </c>
-      <c r="BI36" s="1">
-        <v>8.07</v>
-      </c>
-      <c r="BJ36" s="1">
-        <v>8.07</v>
-      </c>
-      <c r="BK36" s="1">
-        <v>8.61</v>
+      <c r="BG36" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="BH36" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="BI36" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="BJ36" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="BK36" s="1" t="s">
+        <v>394</v>
       </c>
       <c r="BL36" s="1">
         <v>0</v>
       </c>
-      <c r="BM36" s="1">
-        <v>8.07</v>
+      <c r="BM36" s="1" t="s">
+        <v>422</v>
       </c>
       <c r="BN36" s="1">
         <v>0</v>
       </c>
       <c r="BO36" s="1" t="s">
-        <v>137</v>
+        <v>415</v>
       </c>
       <c r="BP36" s="1">
         <v>8.34</v>
@@ -7939,36 +8198,36 @@
       <c r="BF38" s="1">
         <v>-20.59</v>
       </c>
-      <c r="BG38" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH38" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI38" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ38" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK38" s="1">
-        <v>0</v>
+      <c r="BG38" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="BH38" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="BI38" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="BJ38" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="BK38" s="1" t="s">
+        <v>451</v>
       </c>
       <c r="BL38" s="1">
         <v>0</v>
       </c>
-      <c r="BM38" s="1">
-        <v>0</v>
+      <c r="BM38" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="BN38" s="1">
         <v>0</v>
       </c>
       <c r="BO38" s="1" t="s">
-        <v>117</v>
+        <v>450</v>
       </c>
       <c r="BP38" s="1">
         <f>(BH38+BI38)/2</f>
-        <v>0</v>
+        <v>9.14</v>
       </c>
       <c r="BQ38" s="1">
         <v>0</v>
@@ -8268,14 +8527,14 @@
       <c r="BJ40" s="1">
         <v>8.2100000000000009</v>
       </c>
-      <c r="BK40" s="1">
-        <v>9</v>
+      <c r="BK40" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="BL40" s="1">
         <v>0</v>
       </c>
-      <c r="BM40" s="1">
-        <v>8.2100000000000009</v>
+      <c r="BM40" s="1" t="s">
+        <v>454</v>
       </c>
       <c r="BN40" s="1">
         <v>0</v>
@@ -9049,11 +9308,14 @@
       <c r="G45" s="1">
         <v>42.02928</v>
       </c>
-      <c r="N45" s="1">
-        <v>55</v>
-      </c>
-      <c r="O45" s="1">
-        <v>105</v>
+      <c r="M45" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>442</v>
       </c>
       <c r="V45" s="1">
         <v>755.4</v>
@@ -9118,14 +9380,14 @@
       <c r="BJ45" s="1">
         <v>8.4</v>
       </c>
-      <c r="BK45" s="1">
-        <v>9.3000000000000007</v>
+      <c r="BK45" s="1" t="s">
+        <v>455</v>
       </c>
       <c r="BL45" s="1">
         <v>-0.54</v>
       </c>
-      <c r="BM45" s="1">
-        <v>8.59</v>
+      <c r="BM45" s="1" t="s">
+        <v>456</v>
       </c>
       <c r="BN45" s="1">
         <v>-0.63</v>
@@ -9482,11 +9744,14 @@
       <c r="G48" s="1">
         <v>54.349060000000001</v>
       </c>
-      <c r="N48" s="1">
-        <v>21</v>
-      </c>
-      <c r="O48" s="1">
-        <v>29</v>
+      <c r="M48" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>371</v>
       </c>
       <c r="V48" s="1">
         <v>1730.4</v>
@@ -9515,32 +9780,32 @@
       <c r="BE48" s="1">
         <v>0.32</v>
       </c>
-      <c r="BG48" s="1">
-        <v>9.24</v>
-      </c>
-      <c r="BH48" s="1">
-        <v>9.24</v>
-      </c>
-      <c r="BI48" s="1">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="BJ48" s="1">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="BK48" s="1">
-        <v>9.24</v>
-      </c>
-      <c r="BL48" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM48" s="1">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="BN48" s="1">
-        <v>0</v>
+      <c r="BG48" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="BH48" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="BI48" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="BJ48" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="BK48" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="BL48" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="BM48" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="BN48" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="BO48" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="BP48" s="1">
         <v>8.9</v>
@@ -10024,11 +10289,14 @@
       <c r="J51" s="1">
         <v>53</v>
       </c>
-      <c r="N51" s="1">
-        <v>46</v>
-      </c>
-      <c r="O51" s="1">
-        <v>53</v>
+      <c r="M51" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>412</v>
       </c>
       <c r="V51" s="1">
         <v>688.9</v>
@@ -10290,36 +10558,36 @@
       <c r="BF52" s="1">
         <v>-21.82</v>
       </c>
-      <c r="BG52" s="1">
-        <v>9.35</v>
-      </c>
-      <c r="BH52" s="1">
-        <v>9.35</v>
-      </c>
-      <c r="BI52" s="1">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="BJ52" s="1">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="BK52" s="1">
-        <v>9.35</v>
+      <c r="BG52" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="BH52" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="BI52" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="BJ52" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="BK52" s="1" t="s">
+        <v>460</v>
       </c>
       <c r="BL52" s="1">
         <v>0</v>
       </c>
-      <c r="BM52" s="1">
-        <v>8.6300000000000008</v>
+      <c r="BM52" s="1" t="s">
+        <v>461</v>
       </c>
       <c r="BN52" s="1">
         <v>0</v>
       </c>
       <c r="BO52" s="1" t="s">
-        <v>137</v>
+        <v>462</v>
       </c>
       <c r="BP52" s="1">
         <f>(BH52+BI52)/2</f>
-        <v>8.99</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="BQ52" s="1">
         <v>0.36</v>

</xml_diff>

<commit_message>
metadata will be saved into the Google Drive in future
</commit_message>
<xml_diff>
--- a/data/nearby.xlsx
+++ b/data/nearby.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37960" yWindow="0" windowWidth="33600" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="24660" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SGP.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="489">
   <si>
     <t>Galaxy</t>
   </si>
@@ -693,9 +693,6 @@
     <t>IABm</t>
   </si>
   <si>
-    <t>I?</t>
-  </si>
-  <si>
     <t>SABd</t>
   </si>
   <si>
@@ -789,9 +786,6 @@
     <t>HERACLES,THINGS,CAN</t>
   </si>
   <si>
-    <t>STING,CANON</t>
-  </si>
-  <si>
     <t>SGP,CGP,MSC</t>
   </si>
   <si>
@@ -1408,6 +1402,90 @@
   </si>
   <si>
     <t>DorsJr:2008kk</t>
+  </si>
+  <si>
+    <t>CANON,HERACLES</t>
+  </si>
+  <si>
+    <t>STING,HERACLES</t>
+  </si>
+  <si>
+    <t>HERACLES,THINGS,CANON,PAWS</t>
+  </si>
+  <si>
+    <t>CANON,HERACLES,THINGS</t>
+  </si>
+  <si>
+    <t>STING,CANON,HERACLES,THINGS</t>
+  </si>
+  <si>
+    <t>IB(s)m</t>
+  </si>
+  <si>
+    <t>Irr?</t>
+  </si>
+  <si>
+    <t>SAB(rs)bc</t>
+  </si>
+  <si>
+    <t>I0 pec</t>
+  </si>
+  <si>
+    <t>IAB(s)m</t>
+  </si>
+  <si>
+    <t>(R)SA(r)ab</t>
+  </si>
+  <si>
+    <t>SA(s)bc pec</t>
+  </si>
+  <si>
+    <t>AGN</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Emission-Line</t>
+  </si>
+  <si>
+    <t>Interacting</t>
+  </si>
+  <si>
+    <t>HII</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Grand-Design</t>
+  </si>
+  <si>
+    <t>Interacting,Starburst</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Liner</t>
+  </si>
+  <si>
+    <t>Seyfert</t>
+  </si>
+  <si>
+    <t>Group,Emission-Line</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>SF Rings</t>
+  </si>
+  <si>
+    <t>Starburst</t>
+  </si>
+  <si>
+    <t>AGN,Starburst</t>
   </si>
 </sst>
 </file>
@@ -1461,8 +1539,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="185">
+  <cellStyleXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1655,7 +1753,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="185">
+  <cellStyles count="205">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1748,6 +1846,16 @@
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1840,6 +1948,16 @@
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2169,13 +2287,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CE53"/>
+  <dimension ref="A1:CF53"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="BG5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BP52" sqref="BP52"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2186,14 +2304,15 @@
     <col min="4" max="4" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="1"/>
-    <col min="13" max="13" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="16" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.6640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="15.83203125" style="1" customWidth="1"/>
@@ -2205,66 +2324,67 @@
     <col min="24" max="24" width="15.6640625" style="1" customWidth="1"/>
     <col min="25" max="25" width="16.33203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="15.1640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="128.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="108" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="47" width="10.83203125" style="1"/>
-    <col min="48" max="48" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="72.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="142.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="44.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="81" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="16384" width="10.83203125" style="1"/>
+    <col min="27" max="27" width="13.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="128.1640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="108" style="1" customWidth="1"/>
+    <col min="30" max="30" width="22.83203125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="11" style="1" customWidth="1"/>
+    <col min="32" max="32" width="14.1640625" style="1" customWidth="1"/>
+    <col min="33" max="34" width="10.6640625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="11.83203125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="11.33203125" style="1" customWidth="1"/>
+    <col min="37" max="39" width="11.5" style="1" customWidth="1"/>
+    <col min="40" max="41" width="10" style="1" customWidth="1"/>
+    <col min="42" max="42" width="10.1640625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="11.1640625" style="1" customWidth="1"/>
+    <col min="44" max="47" width="10.83203125" style="1" customWidth="1"/>
+    <col min="48" max="48" width="9.5" style="1" customWidth="1"/>
+    <col min="49" max="49" width="12.83203125" style="1" customWidth="1"/>
+    <col min="50" max="50" width="29.1640625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="72.6640625" style="1" customWidth="1"/>
+    <col min="52" max="52" width="142.5" style="1" customWidth="1"/>
+    <col min="53" max="53" width="15.1640625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="15.33203125" style="1" customWidth="1"/>
+    <col min="55" max="55" width="21.6640625" style="1" customWidth="1"/>
+    <col min="56" max="56" width="18.1640625" style="1" customWidth="1"/>
+    <col min="57" max="57" width="18" style="1" customWidth="1"/>
+    <col min="58" max="58" width="44.5" style="1" customWidth="1"/>
+    <col min="59" max="59" width="16.1640625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="18" style="1" customWidth="1"/>
+    <col min="61" max="61" width="16.1640625" style="1" customWidth="1"/>
+    <col min="62" max="62" width="17.83203125" style="1" customWidth="1"/>
+    <col min="63" max="63" width="17.33203125" style="1" customWidth="1"/>
+    <col min="64" max="64" width="17.5" style="1" customWidth="1"/>
+    <col min="65" max="65" width="17.1640625" style="1" customWidth="1"/>
+    <col min="66" max="66" width="17.33203125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="20" style="1" customWidth="1"/>
+    <col min="68" max="68" width="11.6640625" style="1" customWidth="1"/>
+    <col min="69" max="69" width="16.1640625" style="1" customWidth="1"/>
+    <col min="70" max="71" width="14.33203125" style="1" customWidth="1"/>
+    <col min="72" max="72" width="19" style="1" customWidth="1"/>
+    <col min="73" max="73" width="12.5" style="1" customWidth="1"/>
+    <col min="74" max="74" width="17" style="1" customWidth="1"/>
+    <col min="75" max="75" width="13.5" style="1" customWidth="1"/>
+    <col min="76" max="76" width="18.1640625" style="1" customWidth="1"/>
+    <col min="77" max="77" width="13" style="1" customWidth="1"/>
+    <col min="78" max="78" width="18.83203125" style="1" customWidth="1"/>
+    <col min="79" max="79" width="15.5" style="1" customWidth="1"/>
+    <col min="80" max="81" width="12.1640625" style="1" customWidth="1"/>
+    <col min="82" max="82" width="5.1640625" style="1" customWidth="1"/>
+    <col min="83" max="83" width="10.83203125" style="1" customWidth="1"/>
+    <col min="84" max="84" width="18.5" style="1" customWidth="1"/>
+    <col min="85" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83">
+    <row r="1" spans="1:84">
       <c r="A1" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>189</v>
@@ -2504,21 +2624,24 @@
         <v>77</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>474</v>
       </c>
     </row>
-    <row r="2" spans="1:83">
+    <row r="2" spans="1:84">
       <c r="A2" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>191</v>
+        <v>462</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>192</v>
@@ -2728,22 +2851,25 @@
       <c r="CD2" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF2" s="1" t="s">
+        <v>475</v>
+      </c>
     </row>
-    <row r="3" spans="1:83">
+    <row r="3" spans="1:84">
       <c r="A3" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="F3" s="1">
         <v>19.186599999999999</v>
@@ -2752,13 +2878,13 @@
         <v>-72.628600000000006</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="V3" s="1">
         <v>18973</v>
@@ -2812,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="BO3" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BP3" s="1">
         <v>8.02</v>
@@ -2821,24 +2947,24 @@
         <v>0</v>
       </c>
       <c r="BR3" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:83">
+    <row r="4" spans="1:84">
       <c r="A4" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>199</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F4" s="1">
         <v>24.173749999999998</v>
@@ -2907,13 +3033,13 @@
         <v>8.35</v>
       </c>
       <c r="BK4" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="BL4" s="1">
         <v>-0.56999999999999995</v>
       </c>
       <c r="BM4" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="BN4" s="1">
         <v>-0.27</v>
@@ -2931,18 +3057,21 @@
         <v>131</v>
       </c>
       <c r="CE4" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="CF4" s="1" t="s">
+        <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:83">
+    <row r="5" spans="1:84">
       <c r="A5" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>191</v>
@@ -2972,13 +3101,13 @@
         <v>88</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>441</v>
       </c>
       <c r="V5" s="1">
         <v>434.7</v>
@@ -3158,16 +3287,19 @@
       <c r="CD5" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF5" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
-    <row r="6" spans="1:83">
+    <row r="6" spans="1:84">
       <c r="A6" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>219</v>
@@ -3182,13 +3314,13 @@
         <v>33.579149999999998</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="V6" s="1">
         <v>628.29999999999995</v>
@@ -3233,7 +3365,7 @@
         <v>8.91</v>
       </c>
       <c r="BL6" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="BM6" s="1">
         <v>8.32</v>
@@ -3251,18 +3383,21 @@
         <v>0.27</v>
       </c>
       <c r="BR6" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="CF6" s="1" t="s">
+        <v>477</v>
       </c>
     </row>
-    <row r="7" spans="1:83">
+    <row r="7" spans="1:84">
       <c r="A7" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>191</v>
@@ -3469,16 +3604,19 @@
       <c r="CD7" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="CF7" s="1" t="s">
+        <v>478</v>
+      </c>
     </row>
-    <row r="8" spans="1:83">
+    <row r="8" spans="1:84">
       <c r="A8" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>191</v>
@@ -3685,16 +3823,19 @@
       <c r="CD8" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="CF8" s="1" t="s">
+        <v>480</v>
+      </c>
     </row>
-    <row r="9" spans="1:83">
+    <row r="9" spans="1:84">
       <c r="A9" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>191</v>
@@ -3724,7 +3865,7 @@
         <v>88</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="O9" s="1">
         <v>213</v>
@@ -3862,13 +4003,13 @@
         <v>8.5</v>
       </c>
       <c r="BK9" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="BL9" s="1">
         <v>-0.34</v>
       </c>
       <c r="BM9" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="BN9" s="1">
         <v>-0.34</v>
@@ -3915,22 +4056,25 @@
       <c r="CD9" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="CF9" s="1" t="s">
+        <v>473</v>
+      </c>
     </row>
-    <row r="10" spans="1:83">
+    <row r="10" spans="1:84">
       <c r="A10" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F10" s="1">
         <v>79.893900000000002</v>
@@ -3939,13 +4083,13 @@
         <v>-68.506100000000004</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="V10" s="1">
         <v>38739</v>
@@ -3999,7 +4143,7 @@
         <v>-0.03</v>
       </c>
       <c r="BO10" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BP10" s="1">
         <v>8.4499999999999993</v>
@@ -4008,18 +4152,18 @@
         <v>0</v>
       </c>
       <c r="BR10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:83">
+    <row r="11" spans="1:84">
       <c r="A11" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>201</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>219</v>
@@ -4067,31 +4211,31 @@
         <v>0.46</v>
       </c>
       <c r="BG11" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="BH11" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="BI11" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="BJ11" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="BK11" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="BL11" s="1">
         <v>0</v>
       </c>
       <c r="BM11" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="BN11" s="1">
         <v>0</v>
       </c>
       <c r="BO11" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="BP11" s="1">
         <v>8.19</v>
@@ -4099,22 +4243,28 @@
       <c r="BQ11" s="1">
         <v>0.25</v>
       </c>
+      <c r="BR11" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="CF11" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="12" spans="1:83">
+    <row r="12" spans="1:84">
       <c r="A12" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>202</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F12" s="1">
         <v>114.21423799999999</v>
@@ -4207,18 +4357,21 @@
         <v>174</v>
       </c>
       <c r="CE12" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
+      </c>
+      <c r="CF12" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
-    <row r="13" spans="1:83">
+    <row r="13" spans="1:84">
       <c r="A13" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>219</v>
@@ -4301,10 +4454,13 @@
       <c r="BR13" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="CF13" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
-    <row r="14" spans="1:83">
+    <row r="14" spans="1:84">
       <c r="A14" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>197</v>
@@ -4358,25 +4514,25 @@
         <v>0.31</v>
       </c>
       <c r="BG14" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="BH14" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="BI14" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="BJ14" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="BK14" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="BL14" s="1">
         <v>0</v>
       </c>
       <c r="BM14" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="BN14" s="1">
         <v>0</v>
@@ -4391,18 +4547,21 @@
         <v>0.15</v>
       </c>
       <c r="BR14" s="1" t="s">
-        <v>224</v>
+        <v>467</v>
+      </c>
+      <c r="CF14" s="1" t="s">
+        <v>481</v>
       </c>
     </row>
-    <row r="15" spans="1:83">
+    <row r="15" spans="1:84">
       <c r="A15" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>193</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>219</v>
@@ -4450,25 +4609,25 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="BG15" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="BH15" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="BH15" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="BI15" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="BJ15" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="BJ15" s="1" t="s">
-        <v>389</v>
-      </c>
       <c r="BK15" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="BL15" s="1">
         <v>0</v>
       </c>
       <c r="BM15" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="BN15" s="1">
         <v>0</v>
@@ -4485,16 +4644,19 @@
       <c r="BR15" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="CF15" s="1" t="s">
+        <v>481</v>
+      </c>
     </row>
-    <row r="16" spans="1:83">
+    <row r="16" spans="1:84">
       <c r="A16" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>191</v>
@@ -4671,16 +4833,19 @@
       <c r="CD16" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF16" s="1" t="s">
+        <v>482</v>
+      </c>
     </row>
-    <row r="17" spans="1:83">
+    <row r="17" spans="1:84">
       <c r="A17" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>191</v>
@@ -4824,25 +4989,25 @@
         <v>-20.76</v>
       </c>
       <c r="BG17" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="BH17" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="BI17" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="BJ17" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="BK17" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="BL17" s="1">
         <v>0</v>
       </c>
       <c r="BM17" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="BN17" s="1">
         <v>0</v>
@@ -4890,16 +5055,19 @@
       <c r="CD17" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF17" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
-    <row r="18" spans="1:83">
+    <row r="18" spans="1:84">
       <c r="A18" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>203</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>219</v>
@@ -4980,18 +5148,21 @@
         <v>0.34</v>
       </c>
       <c r="BR18" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="CF18" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
-    <row r="19" spans="1:83">
+    <row r="19" spans="1:84">
       <c r="A19" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>204</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>219</v>
@@ -5039,31 +5210,31 @@
         <v>0.42</v>
       </c>
       <c r="BG19" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="BH19" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="BI19" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="BJ19" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="BK19" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL19" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="BH19" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="BI19" s="1" t="s">
+      <c r="BM19" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="BJ19" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="BK19" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="BL19" s="1" t="s">
+      <c r="BN19" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="BM19" s="1" t="s">
+      <c r="BO19" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="BN19" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="BO19" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="BP19" s="1">
         <v>8.8000000000000007</v>
@@ -5071,16 +5242,22 @@
       <c r="BQ19" s="1">
         <v>0.33</v>
       </c>
+      <c r="BR19" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="CF19" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="20" spans="1:83">
+    <row r="20" spans="1:84">
       <c r="A20" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>195</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>219</v>
@@ -5164,21 +5341,21 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:83">
+    <row r="21" spans="1:84">
       <c r="A21" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="F21" s="1">
         <v>146.81442000000001</v>
@@ -5328,13 +5505,13 @@
         <v>8.36</v>
       </c>
       <c r="BK21" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="BL21" s="1">
         <v>0</v>
       </c>
       <c r="BM21" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="BN21" s="1">
         <v>0</v>
@@ -5382,22 +5559,25 @@
       <c r="CD21" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF21" s="1" t="s">
+        <v>481</v>
+      </c>
     </row>
-    <row r="22" spans="1:83">
+    <row r="22" spans="1:84">
       <c r="A22" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="F22" s="1">
         <v>148.88821999999999</v>
@@ -5436,48 +5616,51 @@
         <v>3.63</v>
       </c>
       <c r="BG22" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="BH22" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="BI22" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="BJ22" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK22" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="BH22" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="BI22" s="1" t="s">
+      <c r="BL22" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="BJ22" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="BK22" s="1" t="s">
+      <c r="BM22" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="BL22" s="1" t="s">
+      <c r="BN22" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="BM22" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="BN22" s="1" t="s">
-        <v>395</v>
       </c>
       <c r="BO22" s="1" t="s">
         <v>85</v>
       </c>
       <c r="BR22" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="CE22" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
+      </c>
+      <c r="CF22" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
-    <row r="23" spans="1:83">
+    <row r="23" spans="1:84">
       <c r="A23" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>206</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>219</v>
@@ -5525,31 +5708,31 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="BG23" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="BH23" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="BI23" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BJ23" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BK23" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="BL23" s="1">
         <v>0</v>
       </c>
       <c r="BM23" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BN23" s="1">
         <v>0</v>
       </c>
       <c r="BO23" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="BP23" s="1">
         <v>8.3800000000000008</v>
@@ -5557,16 +5740,22 @@
       <c r="BQ23" s="1">
         <v>0.27</v>
       </c>
+      <c r="BR23" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="CF23" s="1" t="s">
+        <v>484</v>
+      </c>
     </row>
-    <row r="24" spans="1:83">
+    <row r="24" spans="1:84">
       <c r="A24" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>219</v>
@@ -5649,16 +5838,19 @@
       <c r="BR24" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="CF24" s="1" t="s">
+        <v>481</v>
+      </c>
     </row>
-    <row r="25" spans="1:83">
+    <row r="25" spans="1:84">
       <c r="A25" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>191</v>
@@ -5889,22 +6081,25 @@
       <c r="CD25" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="CF25" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
-    <row r="26" spans="1:83">
+    <row r="26" spans="1:84">
       <c r="A26" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F26" s="1">
         <v>154.57025999999999</v>
@@ -6051,27 +6246,30 @@
         <v>0.32</v>
       </c>
       <c r="BR26" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="CE26" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="CF26" s="1" t="s">
+        <v>481</v>
       </c>
     </row>
-    <row r="27" spans="1:83">
+    <row r="27" spans="1:84">
       <c r="A27" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>208</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="F27" s="1">
         <v>154.97897</v>
@@ -6218,13 +6416,13 @@
         <v>8.34</v>
       </c>
       <c r="BK27" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="BL27" s="1">
         <v>-0.66</v>
       </c>
       <c r="BM27" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BN27" s="1">
         <v>-0.5</v>
@@ -6272,22 +6470,25 @@
       <c r="CD27" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF27" s="1" t="s">
+        <v>485</v>
+      </c>
     </row>
-    <row r="28" spans="1:83">
+    <row r="28" spans="1:84">
       <c r="A28" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F28" s="1">
         <v>160.99042</v>
@@ -6431,21 +6632,24 @@
         <v>0.3</v>
       </c>
       <c r="BR28" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="CE28" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="CF28" s="1" t="s">
+        <v>486</v>
       </c>
     </row>
-    <row r="29" spans="1:83">
+    <row r="29" spans="1:84">
       <c r="A29" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>191</v>
@@ -6649,22 +6853,25 @@
       <c r="CD29" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF29" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
-    <row r="30" spans="1:83">
+    <row r="30" spans="1:84">
       <c r="A30" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>210</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F30" s="1">
         <v>166.45241999999999</v>
@@ -6808,21 +7015,24 @@
         <v>0.31</v>
       </c>
       <c r="BR30" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CE30" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="CF30" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
-    <row r="31" spans="1:83">
+    <row r="31" spans="1:84">
       <c r="A31" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>191</v>
@@ -7029,22 +7239,25 @@
       <c r="CD31" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF31" s="1" t="s">
+        <v>481</v>
+      </c>
     </row>
-    <row r="32" spans="1:83">
+    <row r="32" spans="1:84">
       <c r="A32" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>211</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F32" s="1">
         <v>170.06235000000001</v>
@@ -7187,22 +7400,25 @@
       <c r="BR32" s="1" t="s">
         <v>166</v>
       </c>
+      <c r="CF32" s="1" t="s">
+        <v>482</v>
+      </c>
     </row>
-    <row r="33" spans="1:83">
+    <row r="33" spans="1:84">
       <c r="A33" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="F33" s="1">
         <v>178.20604</v>
@@ -7298,45 +7514,48 @@
         <v>1602</v>
       </c>
       <c r="BG33" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="BH33" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="BI33" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="BJ33" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="BK33" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="BL33" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BM33" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="BN33" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO33" s="1" t="s">
         <v>137</v>
       </c>
       <c r="BR33" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="CF33" s="1" t="s">
+        <v>481</v>
       </c>
     </row>
-    <row r="34" spans="1:83">
+    <row r="34" spans="1:84">
       <c r="A34" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>191</v>
@@ -7516,16 +7735,19 @@
       <c r="CD34" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF34" s="1" t="s">
+        <v>481</v>
+      </c>
     </row>
-    <row r="35" spans="1:83">
+    <row r="35" spans="1:84">
       <c r="A35" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>191</v>
@@ -7729,10 +7951,13 @@
       <c r="CD35" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF35" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
-    <row r="36" spans="1:83">
+    <row r="36" spans="1:84">
       <c r="A36" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>212</v>
@@ -7786,31 +8011,31 @@
         <v>0.53</v>
       </c>
       <c r="BG36" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BH36" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BI36" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="BJ36" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="BK36" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BL36" s="1">
         <v>0</v>
       </c>
       <c r="BM36" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="BN36" s="1">
         <v>0</v>
       </c>
       <c r="BO36" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="BP36" s="1">
         <v>8.34</v>
@@ -7818,22 +8043,31 @@
       <c r="BQ36" s="1">
         <v>0.27</v>
       </c>
+      <c r="BR36" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="BS36" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="CF36" s="1" t="s">
+        <v>487</v>
+      </c>
     </row>
-    <row r="37" spans="1:83">
+    <row r="37" spans="1:84">
       <c r="A37" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>256</v>
+        <v>465</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F37" s="1">
         <v>184.70668000000001</v>
@@ -8058,16 +8292,19 @@
       <c r="CD37" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF37" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="38" spans="1:83">
+    <row r="38" spans="1:84">
       <c r="A38" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>191</v>
@@ -8199,31 +8436,31 @@
         <v>-20.59</v>
       </c>
       <c r="BG38" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="BH38" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="BI38" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="BJ38" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="BK38" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="BL38" s="1">
         <v>0</v>
       </c>
       <c r="BM38" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="BN38" s="1">
         <v>0</v>
       </c>
       <c r="BO38" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="BP38" s="1">
         <f>(BH38+BI38)/2</f>
@@ -8265,22 +8502,25 @@
       <c r="CD38" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF38" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="39" spans="1:83">
+    <row r="39" spans="1:84">
       <c r="A39" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="F39" s="1">
         <v>185.72846000000001</v>
@@ -8319,48 +8559,51 @@
         <v>15.85</v>
       </c>
       <c r="BG39" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="BH39" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="BI39" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="BJ39" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="BK39" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="BH39" s="1" t="s">
+      <c r="BL39" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="BM39" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="BN39" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="BI39" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="BJ39" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="BK39" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="BL39" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="BM39" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="BN39" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="BO39" s="1" t="s">
         <v>85</v>
       </c>
       <c r="BR39" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
+      </c>
+      <c r="CF39" s="1" t="s">
+        <v>488</v>
       </c>
     </row>
-    <row r="40" spans="1:83">
+    <row r="40" spans="1:84">
       <c r="A40" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>191</v>
+        <v>462</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>192</v>
@@ -8528,13 +8771,13 @@
         <v>8.2100000000000009</v>
       </c>
       <c r="BK40" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BL40" s="1">
         <v>0</v>
       </c>
       <c r="BM40" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="BN40" s="1">
         <v>0</v>
@@ -8588,16 +8831,19 @@
       <c r="CD40" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF40" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="41" spans="1:83">
+    <row r="41" spans="1:84">
       <c r="A41" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>191</v>
@@ -8802,15 +9048,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:83">
+    <row r="42" spans="1:84">
       <c r="A42" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>191</v>
@@ -9035,22 +9281,25 @@
       <c r="CD42" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF42" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="43" spans="1:83">
+    <row r="43" spans="1:84">
       <c r="A43" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>213</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F43" s="1">
         <v>192.72109</v>
@@ -9193,16 +9442,22 @@
       <c r="BQ43" s="1">
         <v>0.35</v>
       </c>
+      <c r="BR43" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="CF43" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
-    <row r="44" spans="1:83">
+    <row r="44" spans="1:84">
       <c r="A44" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>194</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>219</v>
@@ -9286,21 +9541,21 @@
         <v>222</v>
       </c>
     </row>
-    <row r="45" spans="1:83">
+    <row r="45" spans="1:84">
       <c r="A45" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>214</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F45" s="1">
         <v>198.95554000000001</v>
@@ -9309,13 +9564,13 @@
         <v>42.02928</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="V45" s="1">
         <v>755.4</v>
@@ -9381,13 +9636,13 @@
         <v>8.4</v>
       </c>
       <c r="BK45" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="BL45" s="1">
         <v>-0.54</v>
       </c>
       <c r="BM45" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="BN45" s="1">
         <v>-0.63</v>
@@ -9402,27 +9657,30 @@
         <v>0.37</v>
       </c>
       <c r="BR45" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CE45" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="CF45" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
-    <row r="46" spans="1:83">
+    <row r="46" spans="1:84">
       <c r="A46" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>215</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F46" s="1">
         <v>202.46963</v>
@@ -9437,13 +9695,13 @@
         <v>163</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="V46" s="1">
         <v>828.23</v>
@@ -9455,7 +9713,7 @@
         <v>0.25</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="BA46" s="1">
         <v>-20.72</v>
@@ -9505,16 +9763,22 @@
       <c r="BQ46" s="1">
         <v>0.32</v>
       </c>
+      <c r="BR46" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="CF46" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
-    <row r="47" spans="1:83">
+    <row r="47" spans="1:84">
       <c r="A47" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>191</v>
@@ -9721,16 +9985,19 @@
       <c r="CD47" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF47" s="1" t="s">
+        <v>482</v>
+      </c>
     </row>
-    <row r="48" spans="1:83">
+    <row r="48" spans="1:84">
       <c r="A48" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>219</v>
@@ -9745,13 +10012,13 @@
         <v>54.349060000000001</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="V48" s="1">
         <v>1730.4</v>
@@ -9781,28 +10048,28 @@
         <v>0.32</v>
       </c>
       <c r="BG48" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="BH48" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="BI48" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="BJ48" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="BK48" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="BH48" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="BI48" s="1" t="s">
+      <c r="BL48" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="BJ48" s="1" t="s">
+      <c r="BM48" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="BN48" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="BK48" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="BL48" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="BM48" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="BN48" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="BO48" s="1" t="s">
         <v>113</v>
@@ -9813,19 +10080,25 @@
       <c r="BQ48" s="1">
         <v>0.34</v>
       </c>
+      <c r="BR48" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="CF48" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
-    <row r="49" spans="1:83">
+    <row r="49" spans="1:84">
       <c r="A49" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>191</v>
+        <v>462</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>192</v>
@@ -10056,16 +10329,19 @@
       <c r="CD49" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="CF49" s="1" t="s">
+        <v>481</v>
+      </c>
     </row>
-    <row r="50" spans="1:83">
+    <row r="50" spans="1:84">
       <c r="A50" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>191</v>
@@ -10257,22 +10533,25 @@
       <c r="CD50" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="CF50" s="1" t="s">
+        <v>482</v>
+      </c>
     </row>
-    <row r="51" spans="1:83">
+    <row r="51" spans="1:84">
       <c r="A51" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>217</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="F51" s="1">
         <v>308.71800999999999</v>
@@ -10290,13 +10569,13 @@
         <v>53</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="V51" s="1">
         <v>688.9</v>
@@ -10362,48 +10641,51 @@
         <v>602</v>
       </c>
       <c r="BG51" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="BH51" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="BI51" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="BJ51" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK51" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="BL51" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="BH51" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="BI51" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="BJ51" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="BK51" s="1" t="s">
+      <c r="BM51" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="BL51" s="1" t="s">
+      <c r="BN51" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="BM51" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="BN51" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="BO51" s="1" t="s">
         <v>85</v>
       </c>
       <c r="BR51" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="CE51" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="CF51" s="1" t="s">
+        <v>477</v>
       </c>
     </row>
-    <row r="52" spans="1:83">
+    <row r="52" spans="1:84">
       <c r="A52" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>191</v>
@@ -10559,31 +10841,31 @@
         <v>-21.82</v>
       </c>
       <c r="BG52" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="BH52" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="BI52" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="BJ52" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="BK52" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="BL52" s="1">
         <v>0</v>
       </c>
       <c r="BM52" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="BN52" s="1">
         <v>0</v>
       </c>
       <c r="BO52" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="BP52" s="1">
         <f>(BH52+BI52)/2</f>
@@ -10625,16 +10907,19 @@
       <c r="CD52" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="CF52" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
-    <row r="53" spans="1:83">
+    <row r="53" spans="1:84">
       <c r="A53" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>218</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>219</v>
@@ -10716,6 +11001,9 @@
       </c>
       <c r="BR53" s="1" t="s">
         <v>174</v>
+      </c>
+      <c r="CF53" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>